<commit_message>
Got final dataset. Calculated new figures
</commit_message>
<xml_diff>
--- a/Data/eggCount.xlsx
+++ b/Data/eggCount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alistairseddon/Library/Mobile Documents/com~apple~CloudDocs/BIO201_Rscripts/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF222BA-A3C6-E644-B92E-2BE22C48A246}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96910441-8577-F840-B165-AD4A2BE83C6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="25100" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3740" yWindow="860" windowWidth="25100" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark 1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="136">
   <si>
     <t>ÅMU</t>
   </si>
@@ -375,13 +375,86 @@
   </si>
   <si>
     <t>G6_24_B_015</t>
+  </si>
+  <si>
+    <t>8 on petri dish</t>
+  </si>
+  <si>
+    <r>
+      <t>G</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>5_28_A_005_M3</t>
+    </r>
+  </si>
+  <si>
+    <t>G5_28_A_135_M3</t>
+  </si>
+  <si>
+    <t>G5_24_B_005</t>
+  </si>
+  <si>
+    <t>G5_24_B_015</t>
+  </si>
+  <si>
+    <t>G5_24_B_045</t>
+  </si>
+  <si>
+    <t>G5_24_B_135</t>
+  </si>
+  <si>
+    <t>.+Male 9 on petri dish</t>
+  </si>
+  <si>
+    <t>G5_28_B_135</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (+MALE)</t>
+  </si>
+  <si>
+    <t>G5_28_B_045</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (+MALE) 3 on petri dish</t>
+  </si>
+  <si>
+    <t>G5_28_B_015</t>
+  </si>
+  <si>
+    <t>G5_28_B_005</t>
+  </si>
+  <si>
+    <t>3 on petri dish</t>
+  </si>
+  <si>
+    <t>G5_28_B_005_M5</t>
+  </si>
+  <si>
+    <t>G5_28_A_005_M1</t>
+  </si>
+  <si>
+    <t>G5_28_B_005_M4</t>
+  </si>
+  <si>
+    <t>G5_28_B_135_M2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (+female) 3 on petri dish</t>
+  </si>
+  <si>
+    <t>G5_28_B_135_M3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -398,6 +471,32 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -435,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -448,6 +547,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,10 +770,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I317"/>
+  <dimension ref="A1:I373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A40" sqref="A24:A40"/>
+    <sheetView tabSelected="1" topLeftCell="A348" workbookViewId="0">
+      <selection activeCell="B361" sqref="B361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7974,6 +8078,1147 @@
         <v>5</v>
       </c>
     </row>
+    <row r="318" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A318" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C318" s="12">
+        <v>1</v>
+      </c>
+      <c r="D318" s="11">
+        <v>8</v>
+      </c>
+      <c r="E318" s="11">
+        <v>1</v>
+      </c>
+      <c r="G318" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H318" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A319" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C319" s="12">
+        <v>1</v>
+      </c>
+      <c r="D319" s="11">
+        <v>11</v>
+      </c>
+      <c r="E319" s="11">
+        <v>2</v>
+      </c>
+      <c r="G319" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A320" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C320" s="12">
+        <v>1</v>
+      </c>
+      <c r="D320" s="11">
+        <v>6</v>
+      </c>
+      <c r="E320" s="11">
+        <v>1</v>
+      </c>
+      <c r="G320" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A321" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C321" s="12">
+        <v>1</v>
+      </c>
+      <c r="D321" s="11">
+        <v>13</v>
+      </c>
+      <c r="E321" s="11">
+        <v>1</v>
+      </c>
+      <c r="G321" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A322" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C322" s="12">
+        <v>1</v>
+      </c>
+      <c r="D322" s="11">
+        <v>2</v>
+      </c>
+      <c r="E322" s="11">
+        <v>3</v>
+      </c>
+      <c r="G322" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A323" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C323" s="12">
+        <v>1</v>
+      </c>
+      <c r="D323" s="11">
+        <v>4</v>
+      </c>
+      <c r="E323" s="13">
+        <v>7</v>
+      </c>
+      <c r="G323" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A324" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C324" s="12">
+        <v>1</v>
+      </c>
+      <c r="D324" s="11">
+        <v>1</v>
+      </c>
+      <c r="E324" s="11">
+        <v>2</v>
+      </c>
+      <c r="G324" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A325" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C325" s="12">
+        <v>1</v>
+      </c>
+      <c r="D325" s="11">
+        <v>5</v>
+      </c>
+      <c r="E325" s="11">
+        <v>1</v>
+      </c>
+      <c r="G325" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A326" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C326" s="12">
+        <v>1</v>
+      </c>
+      <c r="D326" s="11">
+        <v>3</v>
+      </c>
+      <c r="E326" s="11">
+        <v>2</v>
+      </c>
+      <c r="G326" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A327" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C327" s="12">
+        <v>1</v>
+      </c>
+      <c r="D327" s="11">
+        <v>1</v>
+      </c>
+      <c r="E327" s="11">
+        <v>20</v>
+      </c>
+      <c r="G327" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A328" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C328" s="12">
+        <v>1</v>
+      </c>
+      <c r="D328" s="11">
+        <v>3</v>
+      </c>
+      <c r="E328" s="11">
+        <v>7</v>
+      </c>
+      <c r="G328" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A329" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C329" s="12">
+        <v>1</v>
+      </c>
+      <c r="D329" s="11">
+        <v>2</v>
+      </c>
+      <c r="E329" s="13">
+        <v>18</v>
+      </c>
+      <c r="G329" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A330" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C330" s="12">
+        <v>1</v>
+      </c>
+      <c r="D330" s="11">
+        <v>0</v>
+      </c>
+      <c r="E330" s="13">
+        <v>71</v>
+      </c>
+      <c r="G330" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A331" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C331" s="12">
+        <v>1</v>
+      </c>
+      <c r="D331" s="11">
+        <v>1</v>
+      </c>
+      <c r="E331" s="11">
+        <v>60</v>
+      </c>
+      <c r="G331" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A332" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C332" s="12">
+        <v>1</v>
+      </c>
+      <c r="D332" s="11">
+        <v>3</v>
+      </c>
+      <c r="E332" s="11">
+        <v>1</v>
+      </c>
+      <c r="G332" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A333" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C333" s="12">
+        <v>1</v>
+      </c>
+      <c r="D333" s="11">
+        <v>2</v>
+      </c>
+      <c r="E333" s="11">
+        <v>4</v>
+      </c>
+      <c r="G333" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A334" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C334" s="12">
+        <v>1</v>
+      </c>
+      <c r="D334" s="11">
+        <v>0</v>
+      </c>
+      <c r="E334" s="11">
+        <v>52</v>
+      </c>
+      <c r="G334" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A335" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C335" s="12">
+        <v>1</v>
+      </c>
+      <c r="D335" s="11">
+        <v>1</v>
+      </c>
+      <c r="E335" s="11">
+        <v>74</v>
+      </c>
+      <c r="G335" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A336" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C336" s="12">
+        <v>1</v>
+      </c>
+      <c r="D336" s="11">
+        <v>2</v>
+      </c>
+      <c r="E336" s="11">
+        <v>8</v>
+      </c>
+      <c r="G336" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A337" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C337" s="12">
+        <v>1</v>
+      </c>
+      <c r="D337" s="11">
+        <v>3</v>
+      </c>
+      <c r="E337" s="11">
+        <v>1</v>
+      </c>
+      <c r="G337" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A338" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C338" s="12">
+        <v>1</v>
+      </c>
+      <c r="D338" s="11">
+        <v>13</v>
+      </c>
+      <c r="E338" s="11">
+        <v>1</v>
+      </c>
+      <c r="G338" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H338" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="339" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A339" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C339" s="12">
+        <v>1</v>
+      </c>
+      <c r="D339" s="11">
+        <v>9</v>
+      </c>
+      <c r="E339" s="11">
+        <v>1</v>
+      </c>
+      <c r="G339" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="340" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A340" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C340" s="12">
+        <v>1</v>
+      </c>
+      <c r="D340" s="11">
+        <v>15</v>
+      </c>
+      <c r="E340" s="14">
+        <v>2</v>
+      </c>
+      <c r="G340" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="341" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A341" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C341" s="12">
+        <v>1</v>
+      </c>
+      <c r="D341" s="11">
+        <v>10</v>
+      </c>
+      <c r="E341" s="11">
+        <v>1</v>
+      </c>
+      <c r="G341" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="342" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A342" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C342" s="12">
+        <v>1</v>
+      </c>
+      <c r="D342" s="4">
+        <v>0</v>
+      </c>
+      <c r="E342" s="4">
+        <v>65</v>
+      </c>
+      <c r="G342" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H342" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="343" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A343" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C343" s="12">
+        <v>1</v>
+      </c>
+      <c r="D343" s="4">
+        <v>1</v>
+      </c>
+      <c r="E343" s="4">
+        <v>67</v>
+      </c>
+      <c r="G343" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="344" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A344" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C344" s="12">
+        <v>1</v>
+      </c>
+      <c r="D344" s="4">
+        <v>2</v>
+      </c>
+      <c r="E344" s="4">
+        <v>2</v>
+      </c>
+      <c r="G344" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="345" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A345" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C345" s="12">
+        <v>1</v>
+      </c>
+      <c r="D345" s="4">
+        <v>0</v>
+      </c>
+      <c r="E345" s="4">
+        <v>2</v>
+      </c>
+      <c r="G345" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="346" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A346" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C346" s="12">
+        <v>1</v>
+      </c>
+      <c r="D346" s="4">
+        <v>1</v>
+      </c>
+      <c r="E346" s="4">
+        <v>24</v>
+      </c>
+      <c r="G346" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="347" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A347" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C347" s="12">
+        <v>1</v>
+      </c>
+      <c r="D347" s="4">
+        <v>2</v>
+      </c>
+      <c r="E347" s="4">
+        <v>18</v>
+      </c>
+      <c r="G347" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="348" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A348" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C348" s="12">
+        <v>1</v>
+      </c>
+      <c r="D348" s="4">
+        <v>3</v>
+      </c>
+      <c r="E348" s="4">
+        <v>2</v>
+      </c>
+      <c r="G348" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="349" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A349" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C349" s="12">
+        <v>1</v>
+      </c>
+      <c r="D349" s="4">
+        <v>3</v>
+      </c>
+      <c r="E349" s="4">
+        <v>2</v>
+      </c>
+      <c r="G349" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H349" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="350" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A350" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C350" s="12">
+        <v>1</v>
+      </c>
+      <c r="D350" s="4">
+        <v>4</v>
+      </c>
+      <c r="E350" s="4">
+        <v>5</v>
+      </c>
+      <c r="G350" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="351" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A351" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C351" s="12">
+        <v>1</v>
+      </c>
+      <c r="D351" s="4">
+        <v>5</v>
+      </c>
+      <c r="E351" s="4">
+        <v>7</v>
+      </c>
+      <c r="G351" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="352" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A352" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C352" s="12">
+        <v>1</v>
+      </c>
+      <c r="D352" s="4">
+        <v>7</v>
+      </c>
+      <c r="E352" s="4">
+        <v>1</v>
+      </c>
+      <c r="G352" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H352" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A353" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C353" s="12">
+        <v>1</v>
+      </c>
+      <c r="D353" s="4">
+        <v>3</v>
+      </c>
+      <c r="E353" s="4">
+        <v>1</v>
+      </c>
+      <c r="G353" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A354" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C354" s="12">
+        <v>1</v>
+      </c>
+      <c r="D354" s="4">
+        <v>6</v>
+      </c>
+      <c r="E354" s="4">
+        <v>1</v>
+      </c>
+      <c r="G354" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="355" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A355" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C355" s="12">
+        <v>1</v>
+      </c>
+      <c r="D355" s="4">
+        <v>10</v>
+      </c>
+      <c r="E355" s="4">
+        <v>3</v>
+      </c>
+      <c r="G355" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A356" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C356" s="12">
+        <v>1</v>
+      </c>
+      <c r="D356" s="4">
+        <v>9</v>
+      </c>
+      <c r="E356" s="4">
+        <v>1</v>
+      </c>
+      <c r="G356" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A357" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C357" s="12">
+        <v>1</v>
+      </c>
+      <c r="D357" s="4">
+        <v>10</v>
+      </c>
+      <c r="E357" s="4">
+        <v>2</v>
+      </c>
+      <c r="G357" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="358" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A358" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C358" s="12">
+        <v>1</v>
+      </c>
+      <c r="D358" s="4">
+        <v>12</v>
+      </c>
+      <c r="E358" s="4">
+        <v>1</v>
+      </c>
+      <c r="G358" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A359" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C359" s="12">
+        <v>1</v>
+      </c>
+      <c r="D359" s="4">
+        <v>15</v>
+      </c>
+      <c r="E359" s="4">
+        <v>1</v>
+      </c>
+      <c r="G359" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H359" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A360" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C360" s="12">
+        <v>1</v>
+      </c>
+      <c r="D360" s="4">
+        <v>9</v>
+      </c>
+      <c r="E360" s="4">
+        <v>3</v>
+      </c>
+      <c r="G360" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A361" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C361" s="12">
+        <v>1</v>
+      </c>
+      <c r="D361" s="4">
+        <v>10</v>
+      </c>
+      <c r="E361" s="4">
+        <v>1</v>
+      </c>
+      <c r="G361" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="362" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A362" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C362" s="12">
+        <v>1</v>
+      </c>
+      <c r="D362" s="4">
+        <v>11</v>
+      </c>
+      <c r="E362" s="4">
+        <v>1</v>
+      </c>
+      <c r="G362" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="363" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A363" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C363" s="12">
+        <v>1</v>
+      </c>
+      <c r="D363" s="4">
+        <v>8</v>
+      </c>
+      <c r="E363" s="4">
+        <v>1</v>
+      </c>
+      <c r="G363" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="364" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A364" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C364" s="12">
+        <v>1</v>
+      </c>
+      <c r="D364" s="4">
+        <v>9</v>
+      </c>
+      <c r="E364" s="4">
+        <v>2</v>
+      </c>
+      <c r="G364" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A365" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C365" s="12">
+        <v>1</v>
+      </c>
+      <c r="D365" s="4">
+        <v>11</v>
+      </c>
+      <c r="E365" s="4">
+        <v>1</v>
+      </c>
+      <c r="G365" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="366" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A366" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C366" s="12">
+        <v>1</v>
+      </c>
+      <c r="D366" s="4">
+        <v>12</v>
+      </c>
+      <c r="E366" s="4">
+        <v>1</v>
+      </c>
+      <c r="G366" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="367" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A367" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C367" s="12">
+        <v>1</v>
+      </c>
+      <c r="D367" s="4">
+        <v>0</v>
+      </c>
+      <c r="E367" s="4">
+        <v>95</v>
+      </c>
+      <c r="G367" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H367" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="368" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A368" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C368" s="12">
+        <v>1</v>
+      </c>
+      <c r="D368" s="4">
+        <v>1</v>
+      </c>
+      <c r="E368" s="4">
+        <v>38</v>
+      </c>
+      <c r="G368" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A369" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C369" s="12">
+        <v>1</v>
+      </c>
+      <c r="D369" s="4">
+        <v>2</v>
+      </c>
+      <c r="E369" s="4">
+        <v>2</v>
+      </c>
+      <c r="G369" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A370" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C370" s="12">
+        <v>1</v>
+      </c>
+      <c r="D370" s="4">
+        <v>0</v>
+      </c>
+      <c r="E370" s="4">
+        <v>92</v>
+      </c>
+      <c r="G370" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A371" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C371" s="12">
+        <v>1</v>
+      </c>
+      <c r="D371" s="4">
+        <v>1</v>
+      </c>
+      <c r="E371" s="4">
+        <v>38</v>
+      </c>
+      <c r="G371" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A372" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C372" s="12">
+        <v>1</v>
+      </c>
+      <c r="D372" s="4">
+        <v>2</v>
+      </c>
+      <c r="E372" s="4">
+        <v>3</v>
+      </c>
+      <c r="G372" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A373" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C373" s="12">
+        <v>1</v>
+      </c>
+      <c r="D373" s="4">
+        <v>3</v>
+      </c>
+      <c r="E373" s="4">
+        <v>2</v>
+      </c>
+      <c r="G373" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A213:E246">
     <sortCondition ref="A212:A246"/>

</xml_diff>